<commit_message>
More pre-fabrication PCB folder tweaks
</commit_message>
<xml_diff>
--- a/pcb/rev2/aqplus_rev2_BOM.xlsx
+++ b/pcb/rev2/aqplus_rev2_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sph\Box\Retro\Aquarius\Aquarius Plus\aqp-gerbers\rev2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A16A181-E687-4A57-915C-1E55ACA3E115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FFFF9B-68E4-4BE7-97CE-C2E758F87926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -558,9 +558,6 @@
     <t>C2798029</t>
   </si>
   <si>
-    <t>C3013947</t>
-  </si>
-  <si>
     <t>C4699785</t>
   </si>
   <si>
@@ -580,6 +577,9 @@
   </si>
   <si>
     <t>PJ-320B-SMT</t>
+  </si>
+  <si>
+    <t>C2913203</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1047,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -1114,7 +1114,7 @@
         <v>124</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E4" s="7"/>
     </row>
@@ -1245,7 +1245,7 @@
         <v>121</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15">
@@ -1368,10 +1368,10 @@
         <v>75</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15">
@@ -1497,7 +1497,7 @@
         <v>109</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15">
@@ -1536,10 +1536,10 @@
         <v>86</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15">
@@ -1609,7 +1609,7 @@
         <v>113</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15">
@@ -1651,7 +1651,7 @@
         <v>116</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15">
@@ -1718,10 +1718,10 @@
         <v>99</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="57">
@@ -1735,7 +1735,7 @@
         <v>121</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15">
@@ -1749,7 +1749,7 @@
         <v>122</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15">
@@ -1774,10 +1774,10 @@
         <v>103</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1785,8 +1785,9 @@
     <hyperlink ref="D41" r:id="rId1" display="https://www.lcsc.com/product-detail/USB-Connectors_MOLEX-676430910_C2798029.html" xr:uid="{5F9E5D26-883F-46FC-97A8-36560CBCF087}"/>
     <hyperlink ref="D48" r:id="rId2" display="https://www.lcsc.com/product-detail/D-Sub-DVI-HDMI-Connectors_TE-Connectivity-5747840-6_C305940.html" xr:uid="{7AE16AA9-D130-4D48-8821-A581FB52A4B6}"/>
     <hyperlink ref="D13" r:id="rId3" display="https://www.lcsc.com/product-detail/D-Sub-DVI-HDMI-Connectors_TE-Connectivity-5747840-6_C305940.html" xr:uid="{8D298D0B-8691-4B0D-BEB7-7C442744ADDD}"/>
+    <hyperlink ref="D49" r:id="rId4" display="https://www.lcsc.com/product-detail/WiFi-Modules_Espressif-Systems-ESP32-S3-WROOM-1-N4R2_C2913203.html" xr:uid="{5EAAE220-0C1D-4F3C-BFB6-B405C9B020EC}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
PCB rev2 Tweaks for LED polarity
</commit_message>
<xml_diff>
--- a/pcb/rev2/aqplus_rev2_BOM.xlsx
+++ b/pcb/rev2/aqplus_rev2_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sph\Box\Retro\Aquarius\Aquarius Plus\aqp-gerbers\rev2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sph\Box\Retro\Aquarius\Aquarius Plus\aquarius-plus\pcb\rev2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FFFF9B-68E4-4BE7-97CE-C2E758F87926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A14AFA-379A-4814-9A2B-955724849332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -558,9 +558,6 @@
     <t>C2798029</t>
   </si>
   <si>
-    <t>C4699785</t>
-  </si>
-  <si>
     <t>C330760</t>
   </si>
   <si>
@@ -580,6 +577,9 @@
   </si>
   <si>
     <t>C2913203</t>
+  </si>
+  <si>
+    <t>C7431259</t>
   </si>
 </sst>
 </file>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -1114,7 +1114,7 @@
         <v>124</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="E4" s="7"/>
     </row>
@@ -1245,7 +1245,7 @@
         <v>121</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15">
@@ -1368,10 +1368,10 @@
         <v>75</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15">
@@ -1497,7 +1497,7 @@
         <v>109</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15">
@@ -1536,10 +1536,10 @@
         <v>86</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15">
@@ -1609,7 +1609,7 @@
         <v>113</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15">
@@ -1651,7 +1651,7 @@
         <v>116</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15">
@@ -1718,10 +1718,10 @@
         <v>99</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="57">
@@ -1735,7 +1735,7 @@
         <v>121</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15">
@@ -1749,7 +1749,7 @@
         <v>122</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15">
@@ -1774,10 +1774,10 @@
         <v>103</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>